<commit_message>
Vanilla Furniture Expanded - Farming 공백 수정
</commit_message>
<xml_diff>
--- a/Data/Vanilla Expanded/Vanilla Furniture Expanded - Farming - 1957158779/Vanilla Furniture Expanded - Farming - 1957158779.xlsx
+++ b/Data/Vanilla Expanded/Vanilla Furniture Expanded - Farming - 1957158779/Vanilla Furniture Expanded - Farming - 1957158779.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\rk_tran\Data\Vanilla Furniture Expanded - Farming - 1957158779\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\RMK\Data\Vanilla Expanded\Vanilla Furniture Expanded - Farming - 1957158779\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C566680-6B6F-4708-81B3-489B81EB37C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B86F333-36AC-4166-8121-2DEC3BF5E519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-3760" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -300,337 +300,359 @@
     <t>VFEF_ScarecrowGizmoText</t>
   </si>
   <si>
+    <t>sprinklers</t>
+  </si>
+  <si>
+    <t>Assemble schematics for a device which can automatically water fields, increasing the speed at which crops grow.</t>
+  </si>
+  <si>
+    <t>farming techniques</t>
+  </si>
+  <si>
+    <t>Develop a theoretical basis for larger-scale farming operations, including centralized feeding and dedicated scarecrows to keep your crops uneaten.</t>
+  </si>
+  <si>
+    <t>Vanilla Expanded</t>
+  </si>
+  <si>
+    <t>planter box</t>
+  </si>
+  <si>
+    <t>Grows plants in a box of soil. Does not require power to work.</t>
+  </si>
+  <si>
+    <t>artificial ecosystem</t>
+  </si>
+  <si>
+    <t>Grows plants quickly in an artificial, sealed ecosystem. Requires a high amount of power to work; plants will die if power is cut.\n\nContains a built-in sun lamp to provide light for the plants.</t>
+  </si>
+  <si>
+    <t>tilable planter box</t>
+  </si>
+  <si>
+    <t>Grows plants in a box of soil. Does not require power to work.\n\nCan be constructed in any desired shape.</t>
+  </si>
+  <si>
+    <t>tilable hydroponics basin</t>
+  </si>
+  <si>
+    <t>An artificial nutrient bath for growing plants. The nutrients pumps must work continuously; the plants will die if power is cut.\n\nThis version is modular and can be assembled in any shape necessary.</t>
+  </si>
+  <si>
+    <t>tilable artificial ecosystem</t>
+  </si>
+  <si>
+    <t>Grows plants quickly in an artificial, sealed ecosystem which can be configured to effectively grow even picky plants. Requires a high amount of power to work; plants will die if power is cut. Contains a built-in sun lamp to provide light for the plants.\n\nThis version is modular and can be assembled in any shape necessary.</t>
+  </si>
+  <si>
+    <t>scarecrow</t>
+  </si>
+  <si>
+    <t>A humanoid figure made out of hay, dressed in old clothes to deter animals in a large radius. Small animals will be too afraid to approach.</t>
+  </si>
+  <si>
+    <t>sprinkler</t>
+  </si>
+  <si>
+    <t>A water sprinkler, providing an area around it with water. Enhances the growth of surrounding plants.</t>
+  </si>
+  <si>
+    <t>Automatically designate the specified area around this {0}.</t>
+  </si>
+  <si>
+    <t>Designate feeding area</t>
+  </si>
+  <si>
+    <t>Scare colony animals</t>
+  </si>
+  <si>
+    <t>Allow to choose if this scarecrow should make your colony animal flee</t>
+  </si>
+  <si>
+    <t>ThingDef+VFEF_Mote_SprinklerWater.label</t>
+  </si>
+  <si>
+    <t>VFEF_Mote_SprinklerWater.label</t>
+  </si>
+  <si>
+    <t>Mote</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.0</t>
+  </si>
+  <si>
+    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.0</t>
+  </si>
+  <si>
+    <t>subject-&gt;pioneering biospheres</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.1</t>
+  </si>
+  <si>
+    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.1</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;conceived and created self-sustaining environments, mastering the balance of nature and technology</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.2</t>
+  </si>
+  <si>
+    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.2</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;ushered in a new age of food security with ecosystems that defy the natural limitations of climate and geography</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.3</t>
+  </si>
+  <si>
+    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.3</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;harnessed the principles of ecological harmony, integrating advanced hydroponics with biodiverse terraria</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.4</t>
+  </si>
+  <si>
+    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.4</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;enabled the cultivation of exotic flora and fauna, previously unseen on this scale</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.5</t>
+  </si>
+  <si>
+    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.5</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;innovated in closed-loop water and nutrient cycles, reducing waste and increasing efficiency</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.6</t>
+  </si>
+  <si>
+    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.6</t>
+  </si>
+  <si>
+    <t>subject_gerund-&gt;revolutionizing agriculture with the creation of artificial ecosystems</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.0</t>
+  </si>
+  <si>
+    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.0</t>
+  </si>
+  <si>
+    <t>subject-&gt;the irrigation evolution</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.1</t>
+  </si>
+  <si>
+    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.1</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;developed automated watering systems, ensuring optimal hydration for crops across vast fields</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.2</t>
+  </si>
+  <si>
+    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.2</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;transformed agricultural productivity with precision irrigation, minimizing water waste</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.3</t>
+  </si>
+  <si>
+    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.3</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;pioneered the use of sprinklers, marking a leap forward from traditional watering methods</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.4</t>
+  </si>
+  <si>
+    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.4</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;empowered farmers to control the very essence of growth - water - with the turn of a valve</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.5</t>
+  </si>
+  <si>
+    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.5</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;fostered greener pastures and bountiful harvests, even in areas once thought barren</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.6</t>
+  </si>
+  <si>
+    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.6</t>
+  </si>
+  <si>
+    <t>subject_gerund-&gt;streamlining growth with the simplicity and efficiency of sprinklers</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.0</t>
+  </si>
+  <si>
+    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.0</t>
+  </si>
+  <si>
+    <t>subject-&gt;cultivating abundance</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.1</t>
+  </si>
+  <si>
+    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.1</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;rediscovered and refined ancient methods for modern largescale farming operations</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.2</t>
+  </si>
+  <si>
+    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.2</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;implemented centralized feeding strategies, optimizing nutrition and yield</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.3</t>
+  </si>
+  <si>
+    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.3</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;crafted scarecrows based on deep understanding of local fauna, effectively protecting crops</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.4</t>
+  </si>
+  <si>
+    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.4</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;laid down the foundational practices for sustainable and efficient food production</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.5</t>
+  </si>
+  <si>
+    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.5</t>
+  </si>
+  <si>
+    <t>subject_story-&gt;inspired a generation of farmers to adopt innovative approaches to agriculture</t>
+  </si>
+  <si>
+    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.6</t>
+  </si>
+  <si>
+    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.6</t>
+  </si>
+  <si>
+    <t>subject_gerund-&gt;advancing the art and science of farming through cutting-edge techniques</t>
+  </si>
+  <si>
+    <t>subject_gerund-&gt;최신 기술을 통해 농업의 예술과 과학을 발전시키고 있습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;농업에 혁신적인 접근 방식을 채택하도록 한 세대의 농민들에게 영감을 주었습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;지속 가능하고 효율적인 식품 생산을 위한 기초적인 실천 방법을 수립했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;지역 생태계에 대한 깊은 이해를 바탕으로 효과적인 작물 보호용 허수아비를 제작했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;영양과 수확량을 최적화하는 중앙 집중식 급여 전략을 도입했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;고대 농법 기술을 재발견하고 현대 대규모 농장 운영에 맞게 정교화했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject-&gt;풍요로움을 키우는</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_gerund-&gt;스프링클러의 단순성과 효율성으로 성장을 최적화했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;한때 불모지로 여겨졌던 지역에서도 녹색 목장과 풍성한 수확을 가능하게 했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;농민들이 밸브를 돌리는 것만으로 성장의 핵심 요소인 물을 통제할 수 있도록 했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;스프링클러의 사용을 선구적으로 도입해 전통적인 관수 방법에서 큰 진전을 이뤘습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;정밀 관개를 통해 농업 생산성을 혁신하고 물 낭비를 최소화했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;광활한 농지에서 작물의 최적 수분을 보장하는 자동화 관개 시스템을 개발했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject-&gt;관개 기술의 진화</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_gerund-&gt;인공 생태계 창조를 통해 농업에 혁명을 일으켰습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;폐쇄형 물과 영양분 순환 시스템을 혁신해 폐기물을 줄이고 효율성을 높였습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;이 규모로 이전에 볼 수 없었던 이국적인 식물과 동물을 재배 가능하게 했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;생태적 조화의 원리를 활용해 고급 수경 재배와 생물 다양성 테라리움을 통합했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;기후와 지리의 자연적 한계를 초월한 생태계를 통해 식량 안보의 새 시대를 열었습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject_story-&gt;자연과 기술의 균형을 마스터하며 자급자족 환경을 구상하고 창조했습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>subject-&gt;선구적인 바이오스피어</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>정착지의 동물도 도망치도록 설정합니다</t>
-  </si>
-  <si>
-    <t>sprinklers</t>
-  </si>
-  <si>
-    <t>Assemble schematics for a device which can automatically water fields, increasing the speed at which crops grow.</t>
-  </si>
-  <si>
-    <t>farming techniques</t>
-  </si>
-  <si>
-    <t>Develop a theoretical basis for larger-scale farming operations, including centralized feeding and dedicated scarecrows to keep your crops uneaten.</t>
-  </si>
-  <si>
-    <t>Vanilla Expanded</t>
-  </si>
-  <si>
-    <t>planter box</t>
-  </si>
-  <si>
-    <t>Grows plants in a box of soil. Does not require power to work.</t>
-  </si>
-  <si>
-    <t>artificial ecosystem</t>
-  </si>
-  <si>
-    <t>Grows plants quickly in an artificial, sealed ecosystem. Requires a high amount of power to work; plants will die if power is cut.\n\nContains a built-in sun lamp to provide light for the plants.</t>
-  </si>
-  <si>
-    <t>tilable planter box</t>
-  </si>
-  <si>
-    <t>Grows plants in a box of soil. Does not require power to work.\n\nCan be constructed in any desired shape.</t>
-  </si>
-  <si>
-    <t>tilable hydroponics basin</t>
-  </si>
-  <si>
-    <t>An artificial nutrient bath for growing plants. The nutrients pumps must work continuously; the plants will die if power is cut.\n\nThis version is modular and can be assembled in any shape necessary.</t>
-  </si>
-  <si>
-    <t>tilable artificial ecosystem</t>
-  </si>
-  <si>
-    <t>Grows plants quickly in an artificial, sealed ecosystem which can be configured to effectively grow even picky plants. Requires a high amount of power to work; plants will die if power is cut. Contains a built-in sun lamp to provide light for the plants.\n\nThis version is modular and can be assembled in any shape necessary.</t>
-  </si>
-  <si>
-    <t>scarecrow</t>
-  </si>
-  <si>
-    <t>A humanoid figure made out of hay, dressed in old clothes to deter animals in a large radius. Small animals will be too afraid to approach.</t>
-  </si>
-  <si>
-    <t>sprinkler</t>
-  </si>
-  <si>
-    <t>A water sprinkler, providing an area around it with water. Enhances the growth of surrounding plants.</t>
-  </si>
-  <si>
-    <t>Automatically designate the specified area around this {0}.</t>
-  </si>
-  <si>
-    <t>Designate feeding area</t>
-  </si>
-  <si>
-    <t>Scare colony animals</t>
-  </si>
-  <si>
-    <t>Allow to choose if this scarecrow should make your colony animal flee</t>
-  </si>
-  <si>
-    <t>ThingDef+VFEF_Mote_SprinklerWater.label</t>
-  </si>
-  <si>
-    <t>VFEF_Mote_SprinklerWater.label</t>
-  </si>
-  <si>
-    <t>Mote</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.0</t>
-  </si>
-  <si>
-    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.0</t>
-  </si>
-  <si>
-    <t>subject-&gt;pioneering biospheres</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.1</t>
-  </si>
-  <si>
-    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.1</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;conceived and created self-sustaining environments, mastering the balance of nature and technology</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.2</t>
-  </si>
-  <si>
-    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.2</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;ushered in a new age of food security with ecosystems that defy the natural limitations of climate and geography</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.3</t>
-  </si>
-  <si>
-    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.3</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;harnessed the principles of ecological harmony, integrating advanced hydroponics with biodiverse terraria</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.4</t>
-  </si>
-  <si>
-    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.4</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;enabled the cultivation of exotic flora and fauna, previously unseen on this scale</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.5</t>
-  </si>
-  <si>
-    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.5</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;innovated in closed-loop water and nutrient cycles, reducing waste and increasing efficiency</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.6</t>
-  </si>
-  <si>
-    <t>VFE_Res_AdvancedHydroponics.generalRules.rulesStrings.6</t>
-  </si>
-  <si>
-    <t>subject_gerund-&gt;revolutionizing agriculture with the creation of artificial ecosystems</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.0</t>
-  </si>
-  <si>
-    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.0</t>
-  </si>
-  <si>
-    <t>subject-&gt;the irrigation evolution</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.1</t>
-  </si>
-  <si>
-    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.1</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;developed automated watering systems, ensuring optimal hydration for crops across vast fields</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.2</t>
-  </si>
-  <si>
-    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.2</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;transformed agricultural productivity with precision irrigation, minimizing water waste</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.3</t>
-  </si>
-  <si>
-    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.3</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;pioneered the use of sprinklers, marking a leap forward from traditional watering methods</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.4</t>
-  </si>
-  <si>
-    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.4</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;empowered farmers to control the very essence of growth - water - with the turn of a valve</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.5</t>
-  </si>
-  <si>
-    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.5</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;fostered greener pastures and bountiful harvests, even in areas once thought barren</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_Sprinkler.generalRules.rulesStrings.6</t>
-  </si>
-  <si>
-    <t>VFE_Res_Sprinkler.generalRules.rulesStrings.6</t>
-  </si>
-  <si>
-    <t>subject_gerund-&gt;streamlining growth with the simplicity and efficiency of sprinklers</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.0</t>
-  </si>
-  <si>
-    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.0</t>
-  </si>
-  <si>
-    <t>subject-&gt;cultivating abundance</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.1</t>
-  </si>
-  <si>
-    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.1</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;rediscovered and refined ancient methods for modern largescale farming operations</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.2</t>
-  </si>
-  <si>
-    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.2</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;implemented centralized feeding strategies, optimizing nutrition and yield</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.3</t>
-  </si>
-  <si>
-    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.3</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;crafted scarecrows based on deep understanding of local fauna, effectively protecting crops</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.4</t>
-  </si>
-  <si>
-    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.4</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;laid down the foundational practices for sustainable and efficient food production</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.5</t>
-  </si>
-  <si>
-    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.5</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;inspired a generation of farmers to adopt innovative approaches to agriculture</t>
-  </si>
-  <si>
-    <t>ResearchProjectDef+VFE_Res_FarmingTechniques.generalRules.rulesStrings.6</t>
-  </si>
-  <si>
-    <t>VFE_Res_FarmingTechniques.generalRules.rulesStrings.6</t>
-  </si>
-  <si>
-    <t>subject_gerund-&gt;advancing the art and science of farming through cutting-edge techniques</t>
-  </si>
-  <si>
-    <t>subject-&gt;선구적인 바이오스피어</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;자연과 기술의 균형을 마스터하며 자급자족 환경을 구상하고 창조했습니다</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;기후와 지리의 자연적 한계를 초월한 생태계를 통해 식량 안보의 새 시대를 열었습니다</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;생태적 조화의 원리를 활용해 고급 수경 재배와 생물 다양성 테라리움을 통합했습니다</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject_story-&gt;이 규모로 이전에 볼 수 없었던 이국적인 식물과 동물을 재배 가능하게 했습니다  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject_story-&gt;폐쇄형 물과 영양분 순환 시스템을 혁신해 폐기물을 줄이고 효율성을 높였습니다  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject_gerund-&gt;인공 생태계 창조를 통해 농업에 혁명을 일으켰습니다  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject-&gt;관개 기술의 진화  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject_story-&gt;광활한 농지에서 작물의 최적 수분을 보장하는 자동화 관개 시스템을 개발했습니다  </t>
-  </si>
-  <si>
-    <t>subject_story-&gt;정밀 관개를 통해 농업 생산성을 혁신하고 물 낭비를 최소화했습니다</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject_story-&gt;스프링클러의 사용을 선구적으로 도입해 전통적인 관수 방법에서 큰 진전을 이뤘습니다  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject_story-&gt;농민들이 밸브를 돌리는 것만으로 성장의 핵심 요소인 물을 통제할 수 있도록 했습니다  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject_story-&gt;한때 불모지로 여겨졌던 지역에서도 녹색 목장과 풍성한 수확을 가능하게 했습니다  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject_gerund-&gt;스프링클러의 단순성과 효율성으로 성장을 최적화했습니다  </t>
-  </si>
-  <si>
-    <t>subject-&gt;풍요로움을 키우는</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;고대 농법 기술을 재발견하고 현대 대규모 농장 운영에 맞게 정교화했습니다</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;영양과 수확량을 최적화하는 중앙 집중식 급여 전략을 도입했습니다</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;지역 생태계에 대한 깊은 이해를 바탕으로 효과적인 작물 보호용 허수아비를 제작했습니다</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;지속 가능하고 효율적인 식품 생산을 위한 기초적인 실천 방법을 수립했습니다</t>
-  </si>
-  <si>
-    <t>subject_story-&gt;농업에 혁신적인 접근 방식을 채택하도록 한 세대의 농민들에게 영감을 주었습니다</t>
-  </si>
-  <si>
-    <t>subject_gerund-&gt;최신 기술을 통해 농업의 예술과 과학을 발전시키고 있습니다</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1002,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1077,7 +1099,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
@@ -1094,7 +1116,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>18</v>
@@ -1111,7 +1133,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>21</v>
@@ -1128,7 +1150,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>24</v>
@@ -1145,7 +1167,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>28</v>
@@ -1162,7 +1184,7 @@
         <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>32</v>
@@ -1179,7 +1201,7 @@
         <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>35</v>
@@ -1196,7 +1218,7 @@
         <v>37</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>38</v>
@@ -1213,7 +1235,7 @@
         <v>40</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>41</v>
@@ -1230,7 +1252,7 @@
         <v>43</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>44</v>
@@ -1247,7 +1269,7 @@
         <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>47</v>
@@ -1264,7 +1286,7 @@
         <v>49</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>50</v>
@@ -1281,7 +1303,7 @@
         <v>52</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>53</v>
@@ -1298,7 +1320,7 @@
         <v>55</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>56</v>
@@ -1315,7 +1337,7 @@
         <v>58</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>59</v>
@@ -1332,7 +1354,7 @@
         <v>61</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>62</v>
@@ -1349,7 +1371,7 @@
         <v>64</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>65</v>
@@ -1366,7 +1388,7 @@
         <v>69</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>15</v>
@@ -1383,7 +1405,7 @@
         <v>71</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>72</v>
@@ -1400,7 +1422,7 @@
         <v>75</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>76</v>
@@ -1417,7 +1439,7 @@
         <v>78</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>79</v>
@@ -1434,7 +1456,7 @@
         <v>81</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>82</v>
@@ -1451,381 +1473,381 @@
         <v>84</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>85</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="F33" s="1" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="F35" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="F36" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="F37" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="F38" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="F39" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="F40" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="F41" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="F42" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="F43" s="1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="F44" s="1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="F45" s="1" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="F47" s="1" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="F48" s="1" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>